<commit_message>
STRUCT finished adding the separate categories blog pages, added images to the blog page to be made as links
</commit_message>
<xml_diff>
--- a/_site/docs/template-full-year.xlsx
+++ b/_site/docs/template-full-year.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nk/Dropbox/Apps/Website/neha-official.github.io/_site/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nk/Dropbox/Apps/Website/neha-official.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -708,7 +708,7 @@
   <dimension ref="B1:AP69"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="11" x14ac:dyDescent="0.15"/>

</xml_diff>